<commit_message>
changes on the dataset
</commit_message>
<xml_diff>
--- a/Business Analysis/data/user_12.xlsx
+++ b/Business Analysis/data/user_12.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usersCode\MScDataScience\Multimodal analysis\Preprocessing\user_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epistimi\Documents\DataSience\Multimodal\emotion_based_music_recomendation\Business Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785AA621-9155-4604-BD4C-3C699A41EFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
-    <sheet name="Template emotion_datasheet3_use" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -376,7 +378,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,8 +903,36 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1210,22 +1240,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>109</v>
       </c>
@@ -1257,7 +1287,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1289,7 +1319,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1321,7 +1351,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1353,7 +1383,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1385,7 +1415,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1417,7 +1447,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1449,7 +1479,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1481,7 +1511,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1513,7 +1543,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1545,7 +1575,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1577,7 +1607,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1609,7 +1639,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1641,7 +1671,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1673,7 +1703,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1705,7 +1735,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1737,7 +1767,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1769,7 +1799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1801,7 +1831,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1833,7 +1863,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1865,7 +1895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1897,7 +1927,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1929,7 +1959,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1961,7 +1991,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1993,7 +2023,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2025,7 +2055,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2057,7 +2087,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2089,7 +2119,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2121,7 +2151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>

</xml_diff>